<commit_message>
resolution de bug+meilleur tuto fct
</commit_message>
<xml_diff>
--- a/Quete/Taverne2.xlsx
+++ b/Quete/Taverne2.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4A8AF2-CA1B-45B0-A033-E2FD177F6229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79574E61-2FCB-4F94-AE37-9966C3880D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -592,22 +581,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="78" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="20" max="20" width="16.109375" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +673,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -695,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -757,7 +746,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -815,7 +804,7 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -873,7 +862,7 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -900,7 +889,7 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -927,7 +916,7 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -954,7 +943,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -981,7 +970,7 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>

</xml_diff>

<commit_message>
plus de resoltuion de bug et ajout  sons
</commit_message>
<xml_diff>
--- a/Quete/Taverne2.xlsx
+++ b/Quete/Taverne2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79574E61-2FCB-4F94-AE37-9966C3880D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE02259-A267-4447-ACBA-A251E493F72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Chap</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Code_init</t>
-  </si>
-  <si>
-    <t>print("Hello World")</t>
   </si>
   <si>
     <t>input_exemple_1</t>
@@ -581,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="78" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,13 +610,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -646,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>19</v>
@@ -667,10 +664,10 @@
         <v>23</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -678,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -690,13 +687,13 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -717,28 +714,26 @@
         <v>18</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1">
         <v>3</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>15</v>
@@ -751,13 +746,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1">
         <v>10</v>
@@ -769,16 +764,16 @@
         <v>126</v>
       </c>
       <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c r="K3" t="s">
-        <v>41</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="1">
         <v>3</v>
@@ -787,19 +782,19 @@
         <v>10</v>
       </c>
       <c r="S3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T3" s="1">
         <v>-10</v>
       </c>
       <c r="U3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V3" s="1">
         <v>127</v>
       </c>
       <c r="W3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="2"/>
@@ -809,55 +804,55 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="Q4" s="1">
         <v>3</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>

</xml_diff>

<commit_message>
Solution bug multi user.py
</commit_message>
<xml_diff>
--- a/Quete/Taverne2.xlsx
+++ b/Quete/Taverne2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8F58DB-129C-4303-BF2A-9FD3168FF270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CE363F-226B-425F-9220-CE89BE363FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Chap</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Écrire un script qui pour une température T donnée affiche l’état de l’eau à cette température c’est-à-dire "Solide", "Liquide" ou "Gazeux". On prendra comme conditions les conditions suivantes : – si la température est strictement négative alors l’eau est à l’état solide ; – si la température est entre 0 et 100 (compris) l’eau est à l’état liquide ; – si la température est strictement supérieure à 100.</t>
+  </si>
+  <si>
+    <t>La moyenne retenue est celle des 2 notes :  11.5</t>
   </si>
 </sst>
 </file>
@@ -578,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="78" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="114" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,7 +843,7 @@
         <v>42</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>43</v>

</xml_diff>